<commit_message>
added more detailed tutorial
</commit_message>
<xml_diff>
--- a/data/output/initialMatch/initialMatchplotData.xlsx
+++ b/data/output/initialMatch/initialMatchplotData.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="4">
   <si>
     <t>uniqueFraction_binDists</t>
   </si>
@@ -47,7 +47,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -57,14 +57,22 @@
     </border>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -84,16 +92,16 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
     </row>
@@ -105,10 +113,10 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>5866.9511423907397</v>
+        <v>1648.095024930298</v>
       </c>
       <c r="D2">
-        <v>165</v>
+        <v>193</v>
       </c>
     </row>
     <row r="3">
@@ -119,10 +127,10 @@
         <v>0</v>
       </c>
       <c r="C3">
-        <v>6057.3598967206835</v>
+        <v>1685.3880516961071</v>
       </c>
       <c r="D3">
-        <v>135</v>
+        <v>193</v>
       </c>
     </row>
     <row r="4">
@@ -133,10 +141,10 @@
         <v>0</v>
       </c>
       <c r="C4">
-        <v>6079.1682153399906</v>
+        <v>1772.5350162972804</v>
       </c>
       <c r="D4">
-        <v>120</v>
+        <v>193</v>
       </c>
     </row>
     <row r="5">
@@ -147,10 +155,10 @@
         <v>0</v>
       </c>
       <c r="C5">
-        <v>6097.5737660154637</v>
+        <v>1908.33304263171</v>
       </c>
       <c r="D5">
-        <v>117</v>
+        <v>192</v>
       </c>
     </row>
     <row r="6">
@@ -161,10 +169,10 @@
         <v>0</v>
       </c>
       <c r="C6">
-        <v>6215.3971038381769</v>
+        <v>1983.3319943973072</v>
       </c>
       <c r="D6">
-        <v>92</v>
+        <v>191</v>
       </c>
     </row>
     <row r="7">
@@ -175,10 +183,10 @@
         <v>0</v>
       </c>
       <c r="C7">
-        <v>6257.8130555650187</v>
+        <v>2166.1340176452613</v>
       </c>
       <c r="D7">
-        <v>92</v>
+        <v>190</v>
       </c>
     </row>
     <row r="8">
@@ -189,10 +197,10 @@
         <v>0</v>
       </c>
       <c r="C8">
-        <v>6411.4290942347634</v>
+        <v>2247.2671919466989</v>
       </c>
       <c r="D8">
-        <v>79</v>
+        <v>188</v>
       </c>
     </row>
     <row r="9">
@@ -203,10 +211,10 @@
         <v>0</v>
       </c>
       <c r="C9">
-        <v>6486.7982403648102</v>
+        <v>2729.2763421830336</v>
       </c>
       <c r="D9">
-        <v>71</v>
+        <v>185</v>
       </c>
     </row>
     <row r="10">
@@ -217,10 +225,10 @@
         <v>0</v>
       </c>
       <c r="C10">
-        <v>6541.3744292770771</v>
+        <v>2986.7329436693867</v>
       </c>
       <c r="D10">
-        <v>67</v>
+        <v>169</v>
       </c>
     </row>
     <row r="11">
@@ -231,10 +239,10 @@
         <v>0</v>
       </c>
       <c r="C11">
-        <v>6605.3989090137475</v>
+        <v>3336.4253853488162</v>
       </c>
       <c r="D11">
-        <v>62</v>
+        <v>167</v>
       </c>
     </row>
     <row r="12">
@@ -245,10 +253,10 @@
         <v>0</v>
       </c>
       <c r="C12">
-        <v>6606.2930658577352</v>
+        <v>3355.2420149968316</v>
       </c>
       <c r="D12">
-        <v>59</v>
+        <v>160</v>
       </c>
     </row>
     <row r="13">
@@ -256,13 +264,13 @@
         <v>27500</v>
       </c>
       <c r="B13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C13">
-        <v>6656.0018603362787</v>
+        <v>3660.6872729584538</v>
       </c>
       <c r="D13">
-        <v>50</v>
+        <v>155</v>
       </c>
     </row>
     <row r="14">
@@ -270,13 +278,13 @@
         <v>30000</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C14">
-        <v>6674.5016113564616</v>
+        <v>3862.7624867185405</v>
       </c>
       <c r="D14">
-        <v>45</v>
+        <v>153</v>
       </c>
     </row>
     <row r="15">
@@ -284,13 +292,13 @@
         <v>32500</v>
       </c>
       <c r="B15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C15">
-        <v>6681.2160839176577</v>
+        <v>4078.4633343454248</v>
       </c>
       <c r="D15">
-        <v>45</v>
+        <v>145</v>
       </c>
     </row>
     <row r="16">
@@ -298,13 +306,13 @@
         <v>35000</v>
       </c>
       <c r="B16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C16">
-        <v>6770.9976261109405</v>
+        <v>4204.7653670567643</v>
       </c>
       <c r="D16">
-        <v>44</v>
+        <v>142</v>
       </c>
     </row>
     <row r="17">
@@ -312,13 +320,13 @@
         <v>37500</v>
       </c>
       <c r="B17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C17">
-        <v>6814.8232591021751</v>
+        <v>4392.4297277930364</v>
       </c>
       <c r="D17">
-        <v>39</v>
+        <v>134</v>
       </c>
     </row>
     <row r="18">
@@ -326,13 +334,13 @@
         <v>40000</v>
       </c>
       <c r="B18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C18">
-        <v>6892.3282663552809</v>
+        <v>4718.8582012177485</v>
       </c>
       <c r="D18">
-        <v>34</v>
+        <v>131</v>
       </c>
     </row>
     <row r="19">
@@ -340,13 +348,13 @@
         <v>42500</v>
       </c>
       <c r="B19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C19">
-        <v>7011.6152877921077</v>
+        <v>5071.9353410705071</v>
       </c>
       <c r="D19">
-        <v>30</v>
+        <v>116</v>
       </c>
     </row>
     <row r="20">
@@ -354,13 +362,13 @@
         <v>45000</v>
       </c>
       <c r="B20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C20">
-        <v>7059.0745361697382</v>
+        <v>5230.9601861226201</v>
       </c>
       <c r="D20">
-        <v>29</v>
+        <v>115</v>
       </c>
     </row>
     <row r="21">
@@ -368,13 +376,13 @@
         <v>47500</v>
       </c>
       <c r="B21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C21">
-        <v>7174.914673889858</v>
+        <v>5731.3549338354542</v>
       </c>
       <c r="D21">
-        <v>27</v>
+        <v>105</v>
       </c>
     </row>
     <row r="22">
@@ -382,13 +390,13 @@
         <v>50000</v>
       </c>
       <c r="B22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C22">
-        <v>7250.4787007755567</v>
+        <v>5775.2100498596592</v>
       </c>
       <c r="D22">
-        <v>26</v>
+        <v>101</v>
       </c>
     </row>
     <row r="23">
@@ -396,13 +404,13 @@
         <v>52500</v>
       </c>
       <c r="B23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C23">
-        <v>7354.1207615866633</v>
+        <v>6202.2744109560326</v>
       </c>
       <c r="D23">
-        <v>26</v>
+        <v>100</v>
       </c>
     </row>
     <row r="24">
@@ -410,13 +418,13 @@
         <v>55000</v>
       </c>
       <c r="B24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C24">
-        <v>7356.5727517098612</v>
+        <v>6367.9254725538367</v>
       </c>
       <c r="D24">
-        <v>26</v>
+        <v>88</v>
       </c>
     </row>
     <row r="25">
@@ -424,13 +432,13 @@
         <v>57500</v>
       </c>
       <c r="B25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C25">
-        <v>7496.346054765615</v>
+        <v>6637.5520770838402</v>
       </c>
       <c r="D25">
-        <v>23</v>
+        <v>86</v>
       </c>
     </row>
     <row r="26">
@@ -438,13 +446,13 @@
         <v>60000</v>
       </c>
       <c r="B26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C26">
-        <v>7710.6927678386983</v>
+        <v>6899.4574655113283</v>
       </c>
       <c r="D26">
-        <v>23</v>
+        <v>78</v>
       </c>
     </row>
     <row r="27">
@@ -455,10 +463,10 @@
         <v>1</v>
       </c>
       <c r="C27">
-        <v>7833.1315857707896</v>
+        <v>7083.029765855852</v>
       </c>
       <c r="D27">
-        <v>21</v>
+        <v>73</v>
       </c>
     </row>
     <row r="28">
@@ -469,10 +477,10 @@
         <v>1</v>
       </c>
       <c r="C28">
-        <v>7987.0203355193726</v>
+        <v>7412.4469824208527</v>
       </c>
       <c r="D28">
-        <v>21</v>
+        <v>71</v>
       </c>
     </row>
     <row r="29">
@@ -483,10 +491,10 @@
         <v>1</v>
       </c>
       <c r="C29">
-        <v>8315.1282191437076</v>
+        <v>7439.8707816735641</v>
       </c>
       <c r="D29">
-        <v>17</v>
+        <v>71</v>
       </c>
     </row>
     <row r="30">
@@ -497,10 +505,10 @@
         <v>1</v>
       </c>
       <c r="C30">
-        <v>8512.3484899527011</v>
+        <v>7796.5191014452084</v>
       </c>
       <c r="D30">
-        <v>17</v>
+        <v>70</v>
       </c>
     </row>
     <row r="31">
@@ -511,10 +519,10 @@
         <v>1</v>
       </c>
       <c r="C31">
-        <v>8823.2676103130871</v>
+        <v>7931.5637343464623</v>
       </c>
       <c r="D31">
-        <v>16</v>
+        <v>67</v>
       </c>
     </row>
     <row r="32">
@@ -525,10 +533,10 @@
         <v>1</v>
       </c>
       <c r="C32">
-        <v>8922.3794126006542</v>
+        <v>8065.5780989585619</v>
       </c>
       <c r="D32">
-        <v>15</v>
+        <v>65</v>
       </c>
     </row>
     <row r="33">
@@ -539,10 +547,10 @@
         <v>1</v>
       </c>
       <c r="C33">
-        <v>9276.7233094449912</v>
+        <v>8427.0334044668416</v>
       </c>
       <c r="D33">
-        <v>15</v>
+        <v>63</v>
       </c>
     </row>
     <row r="34">
@@ -553,10 +561,10 @@
         <v>1</v>
       </c>
       <c r="C34">
-        <v>9462.9395248622423</v>
+        <v>8496.7400227616708</v>
       </c>
       <c r="D34">
-        <v>15</v>
+        <v>61</v>
       </c>
     </row>
     <row r="35">
@@ -567,10 +575,10 @@
         <v>1</v>
       </c>
       <c r="C35">
-        <v>9590.454510689262</v>
+        <v>8945.7729252647587</v>
       </c>
       <c r="D35">
-        <v>15</v>
+        <v>58</v>
       </c>
     </row>
     <row r="36">
@@ -581,10 +589,10 @@
         <v>1</v>
       </c>
       <c r="C36">
-        <v>9891.4342551522823</v>
+        <v>8952.15141033707</v>
       </c>
       <c r="D36">
-        <v>15</v>
+        <v>58</v>
       </c>
     </row>
     <row r="37">
@@ -595,10 +603,10 @@
         <v>1</v>
       </c>
       <c r="C37">
-        <v>10087.869080910994</v>
+        <v>9367.0517653315019</v>
       </c>
       <c r="D37">
-        <v>14</v>
+        <v>57</v>
       </c>
     </row>
     <row r="38">
@@ -609,10 +617,10 @@
         <v>1</v>
       </c>
       <c r="C38">
-        <v>10121.746102644543</v>
+        <v>9409.2816344713592</v>
       </c>
       <c r="D38">
-        <v>14</v>
+        <v>54</v>
       </c>
     </row>
     <row r="39">
@@ -623,10 +631,10 @@
         <v>1</v>
       </c>
       <c r="C39">
-        <v>10348.93036598469</v>
+        <v>9761.367136789806</v>
       </c>
       <c r="D39">
-        <v>14</v>
+        <v>54</v>
       </c>
     </row>
     <row r="40">
@@ -637,10 +645,10 @@
         <v>1</v>
       </c>
       <c r="C40">
-        <v>10511.242858729885</v>
+        <v>9943.2941403540917</v>
       </c>
       <c r="D40">
-        <v>14</v>
+        <v>54</v>
       </c>
     </row>
     <row r="41">
@@ -651,10 +659,10 @@
         <v>1</v>
       </c>
       <c r="C41">
-        <v>10515.748116040057</v>
+        <v>10253.321538311377</v>
       </c>
       <c r="D41">
-        <v>14</v>
+        <v>54</v>
       </c>
     </row>
     <row r="42">
@@ -665,1111 +673,1111 @@
         <v>1</v>
       </c>
       <c r="C42">
-        <v>10882.477042511968</v>
+        <v>10451.704671679161</v>
       </c>
       <c r="D42">
-        <v>14</v>
+        <v>53</v>
       </c>
     </row>
     <row r="43">
       <c r="C43">
-        <v>11019.605977130035</v>
+        <v>10644.861757599298</v>
       </c>
       <c r="D43">
-        <v>14</v>
+        <v>53</v>
       </c>
     </row>
     <row r="44">
       <c r="C44">
-        <v>11387.426204581963</v>
+        <v>10974.825849005532</v>
       </c>
       <c r="D44">
-        <v>13</v>
+        <v>50</v>
       </c>
     </row>
     <row r="45">
       <c r="C45">
-        <v>11843.19530674049</v>
+        <v>11224.899752746123</v>
       </c>
       <c r="D45">
-        <v>13</v>
+        <v>46</v>
       </c>
     </row>
     <row r="46">
       <c r="C46">
-        <v>11927.836415913825</v>
+        <v>11410.834327147162</v>
       </c>
       <c r="D46">
-        <v>11</v>
+        <v>46</v>
       </c>
     </row>
     <row r="47">
       <c r="C47">
-        <v>12472.724002398192</v>
+        <v>11665.496378157255</v>
       </c>
       <c r="D47">
-        <v>10</v>
+        <v>46</v>
       </c>
     </row>
     <row r="48">
       <c r="C48">
-        <v>12879.783380849229</v>
+        <v>11825.246956237321</v>
       </c>
       <c r="D48">
-        <v>8</v>
+        <v>45</v>
       </c>
     </row>
     <row r="49">
       <c r="C49">
-        <v>12968.391798708119</v>
+        <v>12169.440725292186</v>
       </c>
       <c r="D49">
-        <v>8</v>
+        <v>45</v>
       </c>
     </row>
     <row r="50">
       <c r="C50">
-        <v>13446.177480607639</v>
+        <v>12202.497281261734</v>
       </c>
       <c r="D50">
-        <v>8</v>
+        <v>45</v>
       </c>
     </row>
     <row r="51">
       <c r="C51">
-        <v>13928.72650167272</v>
+        <v>12607.946746651494</v>
       </c>
       <c r="D51">
-        <v>6</v>
+        <v>44</v>
       </c>
     </row>
     <row r="52">
       <c r="C52">
-        <v>14154.618386378348</v>
+        <v>12794.148477300081</v>
       </c>
       <c r="D52">
-        <v>6</v>
+        <v>44</v>
       </c>
     </row>
     <row r="53">
       <c r="C53">
-        <v>14344.441010342649</v>
+        <v>12901.90255018228</v>
       </c>
       <c r="D53">
-        <v>6</v>
+        <v>42</v>
       </c>
     </row>
     <row r="54">
       <c r="C54">
-        <v>14550.36427541249</v>
+        <v>13330.120015663775</v>
       </c>
       <c r="D54">
-        <v>5</v>
+        <v>41</v>
       </c>
     </row>
     <row r="55">
       <c r="C55">
-        <v>14775.208815038792</v>
+        <v>13439.668924612688</v>
       </c>
       <c r="D55">
-        <v>5</v>
+        <v>36</v>
       </c>
     </row>
     <row r="56">
       <c r="C56">
-        <v>14932.202284673216</v>
+        <v>13780.425526666439</v>
       </c>
       <c r="D56">
-        <v>5</v>
+        <v>33</v>
       </c>
     </row>
     <row r="57">
       <c r="C57">
-        <v>15137.90067770297</v>
+        <v>13963.259267090903</v>
       </c>
       <c r="D57">
-        <v>5</v>
+        <v>33</v>
       </c>
     </row>
     <row r="58">
       <c r="C58">
-        <v>15267.047081030438</v>
+        <v>14361.015452954573</v>
       </c>
       <c r="D58">
-        <v>5</v>
+        <v>33</v>
       </c>
     </row>
     <row r="59">
       <c r="C59">
-        <v>15583.986474121442</v>
+        <v>14443.557551185235</v>
       </c>
       <c r="D59">
-        <v>5</v>
+        <v>29</v>
       </c>
     </row>
     <row r="60">
       <c r="C60">
-        <v>15808.19016004046</v>
+        <v>14940.862816959399</v>
       </c>
       <c r="D60">
-        <v>4</v>
+        <v>28</v>
       </c>
     </row>
     <row r="61">
       <c r="C61">
-        <v>15894.148251881887</v>
+        <v>15042.134101197211</v>
       </c>
       <c r="D61">
-        <v>4</v>
+        <v>26</v>
       </c>
     </row>
     <row r="62">
       <c r="C62">
-        <v>16409.210739142822</v>
+        <v>15475.170575499322</v>
       </c>
       <c r="D62">
-        <v>4</v>
+        <v>26</v>
       </c>
     </row>
     <row r="63">
       <c r="C63">
-        <v>16666.053151145297</v>
+        <v>15733.9874565604</v>
       </c>
       <c r="D63">
-        <v>4</v>
+        <v>26</v>
       </c>
     </row>
     <row r="64">
       <c r="C64">
-        <v>16850.949585587157</v>
+        <v>15924.585571800604</v>
       </c>
       <c r="D64">
-        <v>4</v>
+        <v>24</v>
       </c>
     </row>
     <row r="65">
       <c r="C65">
-        <v>17108.740987319903</v>
+        <v>16376.151996998564</v>
       </c>
       <c r="D65">
-        <v>4</v>
+        <v>23</v>
       </c>
     </row>
     <row r="66">
       <c r="C66">
-        <v>17313.048501982546</v>
+        <v>16722.002647577832</v>
       </c>
       <c r="D66">
-        <v>4</v>
+        <v>22</v>
       </c>
     </row>
     <row r="67">
       <c r="C67">
-        <v>17406.28475580013</v>
+        <v>17008.583585942717</v>
       </c>
       <c r="D67">
-        <v>4</v>
+        <v>22</v>
       </c>
     </row>
     <row r="68">
       <c r="C68">
-        <v>17704.836411195669</v>
+        <v>17258.875254430692</v>
       </c>
       <c r="D68">
-        <v>3</v>
+        <v>22</v>
       </c>
     </row>
     <row r="69">
       <c r="C69">
-        <v>17744.400632357239</v>
+        <v>17605.488300731678</v>
       </c>
       <c r="D69">
-        <v>3</v>
+        <v>19</v>
       </c>
     </row>
     <row r="70">
       <c r="C70">
-        <v>17902.450427715197</v>
+        <v>17779.002175510304</v>
       </c>
       <c r="D70">
-        <v>3</v>
+        <v>15</v>
       </c>
     </row>
     <row r="71">
       <c r="C71">
-        <v>18111.334162010262</v>
+        <v>18114.307294423379</v>
       </c>
       <c r="D71">
-        <v>3</v>
+        <v>14</v>
       </c>
     </row>
     <row r="72">
       <c r="C72">
-        <v>18143.517614972025</v>
+        <v>18505.485833168499</v>
       </c>
       <c r="D72">
-        <v>3</v>
+        <v>12</v>
       </c>
     </row>
     <row r="73">
       <c r="C73">
-        <v>18506.266721908014</v>
+        <v>19254.426974303857</v>
       </c>
       <c r="D73">
-        <v>3</v>
+        <v>12</v>
       </c>
     </row>
     <row r="74">
       <c r="C74">
-        <v>18515.037048928636</v>
+        <v>19320.010249479685</v>
       </c>
       <c r="D74">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="75">
       <c r="C75">
-        <v>18894.214835149938</v>
+        <v>19748.404896031479</v>
       </c>
       <c r="D75">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="76">
       <c r="C76">
-        <v>18939.606894716693</v>
+        <v>20264.887717626269</v>
       </c>
       <c r="D76">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="77">
       <c r="C77">
-        <v>19159.970629789601</v>
+        <v>20350.383685542638</v>
       </c>
       <c r="D77">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="78">
       <c r="C78">
-        <v>19427.951135907257</v>
+        <v>20823.395467291113</v>
       </c>
       <c r="D78">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="79">
       <c r="C79">
-        <v>19494.946919527636</v>
+        <v>21290.066784639264</v>
       </c>
       <c r="D79">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="80">
       <c r="C80">
-        <v>19929.127480951091</v>
+        <v>21527.83825877554</v>
       </c>
       <c r="D80">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="81">
       <c r="C81">
-        <v>19974.46716626003</v>
+        <v>21941.226391320972</v>
       </c>
       <c r="D81">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="82">
       <c r="C82">
-        <v>20300.373975077408</v>
+        <v>22088.186141808928</v>
       </c>
       <c r="D82">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="83">
       <c r="C83">
-        <v>20674.97910333164</v>
+        <v>22275.599338073935</v>
       </c>
       <c r="D83">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="84">
       <c r="C84">
-        <v>20730.911504977295</v>
+        <v>22553.649265269691</v>
       </c>
       <c r="D84">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="85">
       <c r="C85">
-        <v>21214.729028747926</v>
+        <v>22600.703350081829</v>
       </c>
       <c r="D85">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="86">
       <c r="C86">
-        <v>21305.050232205511</v>
+        <v>23106.528783527829</v>
       </c>
       <c r="D86">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="87">
       <c r="C87">
-        <v>21835.702192986606</v>
+        <v>23213.653151746716</v>
       </c>
       <c r="D87">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="88">
       <c r="C88">
-        <v>21836.888431862266</v>
+        <v>23921.506170406581</v>
       </c>
       <c r="D88">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="89">
       <c r="C89">
-        <v>22326.330845994376</v>
+        <v>24138.455517982089</v>
       </c>
       <c r="D89">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="90">
       <c r="C90">
-        <v>22562.390625286142</v>
+        <v>24343.572370118563</v>
       </c>
       <c r="D90">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="91">
       <c r="C91">
-        <v>22949.472068873394</v>
+        <v>24609.15816276534</v>
       </c>
       <c r="D91">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="92">
       <c r="C92">
-        <v>23308.24629394498</v>
+        <v>24790.253888106916</v>
       </c>
       <c r="D92">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="93">
       <c r="C93">
-        <v>23574.265973319296</v>
+        <v>24876.184750463646</v>
       </c>
       <c r="D93">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="94">
       <c r="C94">
-        <v>24004.283585493649</v>
+        <v>25054.10390376794</v>
       </c>
       <c r="D94">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="95">
       <c r="C95">
-        <v>24259.670939268733</v>
+        <v>25296.488582030513</v>
       </c>
       <c r="D95">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="96">
       <c r="C96">
-        <v>24593.696383943588</v>
+        <v>25530.459673918915</v>
       </c>
       <c r="D96">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="97">
       <c r="C97">
-        <v>25003.356727767576</v>
+        <v>25680.326301883317</v>
       </c>
       <c r="D97">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="98">
       <c r="C98">
-        <v>25273.558815489363</v>
+        <v>26066.79316641769</v>
       </c>
       <c r="D98">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="99">
       <c r="C99">
-        <v>25441.429112720853</v>
+        <v>26374.75068102825</v>
       </c>
       <c r="D99">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="100">
       <c r="C100">
-        <v>25821.760923128386</v>
+        <v>26572.341479576091</v>
       </c>
       <c r="D100">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="101">
       <c r="C101">
-        <v>25929.600894730331</v>
+        <v>27025.777382787714</v>
       </c>
       <c r="D101">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="102">
       <c r="C102">
-        <v>26439.565741335464</v>
+        <v>27277.891700114949</v>
       </c>
       <c r="D102">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="103">
       <c r="C103">
-        <v>26552.018756305519</v>
+        <v>27726.710381348883</v>
       </c>
       <c r="D103">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="104">
       <c r="C104">
-        <v>27112.267972974892</v>
+        <v>28149.301961647288</v>
       </c>
       <c r="D104">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="105">
       <c r="C105">
-        <v>27172.119121452415</v>
+        <v>28241.737376358418</v>
       </c>
       <c r="D105">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="106">
       <c r="C106">
-        <v>27651.365290560247</v>
+        <v>28875.974438913749</v>
       </c>
       <c r="D106">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="107">
       <c r="C107">
-        <v>27980.853863082881</v>
+        <v>29092.185468541207</v>
       </c>
       <c r="D107">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="108">
       <c r="C108">
-        <v>28374.304040804243</v>
+        <v>29610.227045262589</v>
       </c>
       <c r="D108">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="109">
       <c r="C109">
-        <v>28502.167551202139</v>
+        <v>29750.68623507028</v>
       </c>
       <c r="D109">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="110">
       <c r="C110">
-        <v>28894.561858951936</v>
+        <v>30314.393301981156</v>
       </c>
       <c r="D110">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="111">
       <c r="C111">
-        <v>29180.716789715774</v>
+        <v>30697.333499442586</v>
       </c>
       <c r="D111">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="112">
       <c r="C112">
-        <v>29282.047937833857</v>
+        <v>30955.303591417094</v>
       </c>
       <c r="D112">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="113">
       <c r="C113">
-        <v>29855.990656697359</v>
+        <v>31540.273921981083</v>
       </c>
       <c r="D113">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="114">
       <c r="C114">
-        <v>30062.640382933761</v>
+        <v>31547.182368332044</v>
       </c>
       <c r="D114">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="115">
       <c r="C115">
-        <v>30489.07055443967</v>
+        <v>31947.958386651251</v>
       </c>
       <c r="D115">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="116">
       <c r="C116">
-        <v>30729.062427298366</v>
+        <v>32210.827308592994</v>
       </c>
       <c r="D116">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="117">
       <c r="C117">
-        <v>31066.701257262575</v>
+        <v>32369.262985097452</v>
       </c>
       <c r="D117">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="118">
       <c r="C118">
-        <v>31459.080527593302</v>
+        <v>32738.266429656902</v>
       </c>
       <c r="D118">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="119">
       <c r="C119">
-        <v>31940.462318557635</v>
+        <v>32755.933441793411</v>
       </c>
       <c r="D119">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="120">
       <c r="C120">
-        <v>32286.002594040656</v>
+        <v>33372.298764310501</v>
       </c>
       <c r="D120">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="121">
       <c r="C121">
-        <v>32600.384591841859</v>
+        <v>33633.479905713</v>
       </c>
       <c r="D121">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="122">
       <c r="C122">
-        <v>33125.217428949807</v>
+        <v>34111.368806754152</v>
       </c>
       <c r="D122">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="123">
       <c r="C123">
-        <v>33278.095593612321</v>
+        <v>34276.394555530489</v>
       </c>
       <c r="D123">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="124">
       <c r="C124">
-        <v>33894.238444667848</v>
+        <v>34595.63577239187</v>
       </c>
       <c r="D124">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="125">
       <c r="C125">
-        <v>34022.78663973308</v>
+        <v>35019.017483418924</v>
       </c>
       <c r="D125">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="126">
       <c r="C126">
-        <v>34652.193694668167</v>
+        <v>35325.266335018619</v>
       </c>
       <c r="D126">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="127">
       <c r="C127">
-        <v>34823.027728788889</v>
+        <v>35586.952612057132</v>
       </c>
       <c r="D127">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="128">
       <c r="C128">
-        <v>35444.716813652216</v>
+        <v>35864.71331162149</v>
       </c>
       <c r="D128">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="129">
       <c r="C129">
-        <v>35501.062182667156</v>
+        <v>36256.196012819659</v>
       </c>
       <c r="D129">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="130">
       <c r="C130">
-        <v>36230.079492510085</v>
+        <v>36263.24514162515</v>
       </c>
       <c r="D130">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="131">
       <c r="C131">
-        <v>36437.24464368842</v>
+        <v>36686.336348455407</v>
       </c>
       <c r="D131">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="132">
       <c r="C132">
-        <v>37116.463498776393</v>
+        <v>36870.929753354474</v>
       </c>
       <c r="D132">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="133">
       <c r="C133">
-        <v>37297.414952846266</v>
+        <v>37207.798143292493</v>
       </c>
       <c r="D133">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="134">
       <c r="C134">
-        <v>37759.897282741644</v>
+        <v>37515.144661237813</v>
       </c>
       <c r="D134">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="135">
       <c r="C135">
-        <v>37807.86308510969</v>
+        <v>37770.700876525974</v>
       </c>
       <c r="D135">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="136">
       <c r="C136">
-        <v>38164.417538309164</v>
+        <v>38124.050790859044</v>
       </c>
       <c r="D136">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="137">
       <c r="C137">
-        <v>38514.435159072505</v>
+        <v>38218.803997801915</v>
       </c>
       <c r="D137">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="138">
       <c r="C138">
-        <v>38517.066930845089</v>
+        <v>38788.131671097537</v>
       </c>
       <c r="D138">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="139">
       <c r="C139">
-        <v>39171.906241284712</v>
+        <v>38974.637757844524</v>
       </c>
       <c r="D139">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="140">
       <c r="C140">
-        <v>39329.502542188347</v>
+        <v>39366.51074063842</v>
       </c>
       <c r="D140">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="141">
       <c r="C141">
-        <v>39913.969478627405</v>
+        <v>39576.43080764106</v>
       </c>
       <c r="D141">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="142">
       <c r="C142">
-        <v>39970.975054786941</v>
+        <v>39927.501009705076</v>
       </c>
       <c r="D142">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="143">
       <c r="C143">
-        <v>40707.778490504737</v>
+        <v>40245.850590211157</v>
       </c>
       <c r="D143">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="144">
       <c r="C144">
-        <v>40730.158831509609</v>
+        <v>40576.52847749299</v>
       </c>
       <c r="D144">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="145">
       <c r="C145">
-        <v>41314.062701661285</v>
+        <v>40961.333903436294</v>
       </c>
       <c r="D145">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="146">
       <c r="C146">
-        <v>41568.237047919174</v>
+        <v>41309.30226631285</v>
       </c>
       <c r="D146">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="147">
       <c r="C147">
-        <v>41997.723864514373</v>
+        <v>41576.769972627742</v>
       </c>
       <c r="D147">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="148">
       <c r="C148">
-        <v>42431.555913777192</v>
+        <v>41958.258372625525</v>
       </c>
       <c r="D148">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="149">
       <c r="C149">
-        <v>42595.638969302956</v>
+        <v>42354.953269718055</v>
       </c>
       <c r="D149">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="150">
       <c r="C150">
-        <v>42936.56227375452</v>
+        <v>42484.099815135545</v>
       </c>
       <c r="D150">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="151">
       <c r="C151">
-        <v>43517.193136690243</v>
+        <v>43131.500887421018</v>
       </c>
       <c r="D151">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="152">
       <c r="C152">
-        <v>43594.903057196949</v>
+        <v>43998.822044232045</v>
       </c>
       <c r="D152">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="153">
       <c r="C153">
-        <v>43986.314014229472</v>
+        <v>44683.700266007516</v>
       </c>
       <c r="D153">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="154">
       <c r="C154">
-        <v>44410.360879920801</v>
+        <v>45354.005383851167</v>
       </c>
       <c r="D154">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="155">
       <c r="C155">
-        <v>44614.519727711966</v>
+        <v>45961.79576631009</v>
       </c>
       <c r="D155">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="156">
       <c r="C156">
-        <v>45224.852862876178</v>
+        <v>46681.668151050471</v>
       </c>
       <c r="D156">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="157">
       <c r="C157">
-        <v>45345.185070046849</v>
+        <v>47458.496750318591</v>
       </c>
       <c r="D157">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="158">
       <c r="C158">
-        <v>45800.146685354623</v>
+        <v>48267.754228014383</v>
       </c>
       <c r="D158">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="159">
       <c r="C159">
-        <v>46171.360459245734</v>
+        <v>49289.282251166936</v>
       </c>
       <c r="D159">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="160">
       <c r="C160">
-        <v>46467.937159172448</v>
+        <v>50271.522325133541</v>
       </c>
       <c r="D160">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="161">
       <c r="C161">
-        <v>47093.862413949442</v>
+        <v>51091.092809420312</v>
       </c>
       <c r="D161">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="162">
       <c r="C162">
-        <v>47177.309213324152</v>
+        <v>52025.515007742113</v>
       </c>
       <c r="D162">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="163">
       <c r="C163">
-        <v>47785.124899148272</v>
+        <v>52855.090506190601</v>
       </c>
       <c r="D163">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="164">
       <c r="C164">
-        <v>47820.263010234477</v>
+        <v>53773.657829461452</v>
       </c>
       <c r="D164">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="165">
       <c r="C165">
-        <v>48407.833372527632</v>
+        <v>54462.157877733785</v>
       </c>
       <c r="D165">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="166">
       <c r="C166">
-        <v>48474.417511673106</v>
+        <v>55148.473341915822</v>
       </c>
       <c r="D166">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="167">
       <c r="C167">
-        <v>49110.796368000389</v>
+        <v>55771.556372860883</v>
       </c>
       <c r="D167">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="168">
       <c r="C168">
-        <v>49800.122448315327</v>
+        <v>56458.169081145374</v>
       </c>
       <c r="D168">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="169">
       <c r="C169">
-        <v>50244.167455433075</v>
+        <v>56896.411358974125</v>
       </c>
       <c r="D169">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="170">
       <c r="C170">
-        <v>50784.599609960496</v>
+        <v>57427.854865108799</v>
       </c>
       <c r="D170">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="171">
       <c r="C171">
-        <v>51335.614478480726</v>
+        <v>57969.598943680816</v>
       </c>
       <c r="D171">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="172">
       <c r="C172">
-        <v>52016.397521919949</v>
+        <v>58648.788072920994</v>
       </c>
       <c r="D172">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="173">
       <c r="C173">
-        <v>52605.450639339644</v>
+        <v>59243.162531721748</v>
       </c>
       <c r="D173">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="174">
       <c r="C174">
-        <v>53251.128722835536</v>
+        <v>59876.068991476051</v>
       </c>
       <c r="D174">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="175">
       <c r="C175">
-        <v>53624.447668129877</v>
+        <v>60224.50033931373</v>
       </c>
       <c r="D175">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="176">
       <c r="C176">
-        <v>54305.292460238161</v>
+        <v>60904.182828899364</v>
       </c>
       <c r="D176">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="177">
       <c r="C177">
-        <v>54931.572545937554</v>
+        <v>61542.259725570686</v>
       </c>
       <c r="D177">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="178">
       <c r="C178">
-        <v>55577.620716371079</v>
+        <v>62176.249903615128</v>
       </c>
       <c r="D178">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="179">
       <c r="C179">
-        <v>56427.465311438544</v>
+        <v>63007.635113481287</v>
       </c>
       <c r="D179">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="180">
       <c r="C180">
-        <v>57147.934333888225</v>
+        <v>63736.198031624073</v>
       </c>
       <c r="D180">
         <v>1</v>
@@ -1777,7 +1785,7 @@
     </row>
     <row r="181">
       <c r="C181">
-        <v>57904.698355971079</v>
+        <v>64478.844741884139</v>
       </c>
       <c r="D181">
         <v>1</v>
@@ -1785,7 +1793,7 @@
     </row>
     <row r="182">
       <c r="C182">
-        <v>58512.024699817048</v>
+        <v>65066.110714626244</v>
       </c>
       <c r="D182">
         <v>1</v>
@@ -1793,7 +1801,7 @@
     </row>
     <row r="183">
       <c r="C183">
-        <v>59201.92868313667</v>
+        <v>65754.745597828907</v>
       </c>
       <c r="D183">
         <v>1</v>

</xml_diff>